<commit_message>
Gantt chart edited to reflect actual timeline achieved
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\2023\Tri2\Software Technologies\Assignment\2810ICT-7810ICT-2023-Assignment-main\Assignment Repo Clone\SoftwareTechnologies2810ICT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68EA6986-B985-45AE-8F94-3098FA81AA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF4D26-D7CE-45CC-8E88-11091ABAF613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1115D2F1-A1D8-42E5-8CFC-D43F326BF41C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{1115D2F1-A1D8-42E5-8CFC-D43F326BF41C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Victoria Accident Data Visualisation Project</t>
   </si>
@@ -123,13 +123,22 @@
   </si>
   <si>
     <t>Week 10</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +166,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,13 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -208,6 +228,11 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,24 +547,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC0A6F8-92C6-419E-9ACD-11233FB58D6D}">
-  <dimension ref="B2:L20"/>
+  <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:12" ht="33.4" x14ac:dyDescent="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
@@ -573,148 +598,165 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="7"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B22" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B23" s="6"/>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B24" s="9"/>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -725,6 +767,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>